<commit_message>
UI changes white background
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/report template - All DB.xlsx
+++ b/src/main/resources/templates/report template - All DB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\extent-excel-report\src\main\resources\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Excel Extent\White Back - Jan 30\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -634,7 +634,7 @@
             <a:r>
               <a:rPr lang="en-US" sz="1400" b="0" i="1">
                 <a:solidFill>
-                  <a:schemeClr val="bg1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:rPr>
               <a:t>Tags with</a:t>
@@ -642,14 +642,14 @@
             <a:r>
               <a:rPr lang="en-US" sz="1400" b="0" i="1" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="bg1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:rPr>
               <a:t> Failed &amp; Skipped Scenarios</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1400" b="0" i="1">
               <a:solidFill>
-                <a:schemeClr val="bg1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:endParaRPr>
           </a:p>
@@ -954,7 +954,7 @@
                 <a:r>
                   <a:rPr lang="en-US" sz="1100">
                     <a:solidFill>
-                      <a:schemeClr val="bg1"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:t>Scenarios</a:t>
@@ -975,9 +975,7 @@
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="tx2"/>
-        </a:solidFill>
+        <a:noFill/>
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -985,9 +983,7 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="tx2"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="6350">
       <a:solidFill>
         <a:schemeClr val="tx1"/>
@@ -1028,7 +1024,7 @@
             <a:r>
               <a:rPr lang="en-US" sz="1400" b="0" i="1">
                 <a:solidFill>
-                  <a:schemeClr val="bg1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
@@ -1330,7 +1326,7 @@
                 <a:r>
                   <a:rPr lang="en-US" sz="1100">
                     <a:solidFill>
-                      <a:schemeClr val="bg1"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:t>Scenarios</a:t>
@@ -1352,9 +1348,7 @@
         <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="tx2"/>
-        </a:solidFill>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -1365,9 +1359,7 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="tx2"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln>
       <a:noFill/>
     </a:ln>
@@ -1599,7 +1591,7 @@
             <a:r>
               <a:rPr lang="en-US" sz="1400" b="0" i="1">
                 <a:solidFill>
-                  <a:schemeClr val="bg1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
@@ -1608,7 +1600,7 @@
             <a:r>
               <a:rPr lang="en-US" sz="1400" b="0" i="1" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="bg1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
@@ -1617,7 +1609,7 @@
             <a:r>
               <a:rPr lang="en-US" sz="1400" b="0" i="1">
                 <a:solidFill>
-                  <a:schemeClr val="bg1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
@@ -1626,6 +1618,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1685,6 +1678,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -1758,6 +1752,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -1831,6 +1826,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -1919,7 +1915,7 @@
                 <a:r>
                   <a:rPr lang="en-US" sz="1100">
                     <a:solidFill>
-                      <a:schemeClr val="bg1"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:t>Scenarios</a:t>
@@ -1927,6 +1923,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:ln>
@@ -1945,9 +1942,7 @@
         <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="tx2"/>
-        </a:solidFill>
+        <a:noFill/>
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -1955,9 +1950,7 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="tx2"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="6350">
       <a:solidFill>
         <a:schemeClr val="tx1"/>
@@ -1998,7 +1991,7 @@
             <a:r>
               <a:rPr lang="en-US" sz="1400" b="0" i="1">
                 <a:solidFill>
-                  <a:schemeClr val="bg1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:rPr>
               <a:t>Scenarios with Failed &amp; Skipped Steps</a:t>
@@ -2006,6 +1999,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2065,6 +2059,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2138,6 +2133,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2211,6 +2207,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2294,7 +2291,7 @@
                 <a:r>
                   <a:rPr lang="en-US" sz="1100">
                     <a:solidFill>
-                      <a:schemeClr val="bg1"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:t>Steps</a:t>
@@ -2302,6 +2299,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2313,9 +2311,7 @@
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="tx2"/>
-        </a:solidFill>
+        <a:noFill/>
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -2323,9 +2319,7 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="tx2"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="6350">
       <a:solidFill>
         <a:schemeClr val="tx1"/>
@@ -2366,7 +2360,7 @@
             <a:r>
               <a:rPr lang="en-US" sz="1600" b="0" i="1">
                 <a:solidFill>
-                  <a:schemeClr val="bg1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:rPr>
               <a:t>Features</a:t>
@@ -2620,7 +2614,7 @@
             <a:r>
               <a:rPr lang="en-US" sz="1800" b="0" i="1">
                 <a:solidFill>
-                  <a:schemeClr val="bg1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:rPr>
               <a:t>Scenarios</a:t>
@@ -2874,7 +2868,7 @@
             <a:r>
               <a:rPr lang="en-US" sz="1600" b="0" i="1">
                 <a:solidFill>
-                  <a:schemeClr val="bg1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:rPr>
               <a:t>Steps</a:t>
@@ -3128,7 +3122,7 @@
             <a:r>
               <a:rPr lang="en-US" sz="1400" b="0" i="1">
                 <a:solidFill>
-                  <a:schemeClr val="bg1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:rPr>
               <a:t>Scenarios</a:t>
@@ -3428,7 +3422,7 @@
                 <a:r>
                   <a:rPr lang="en-US" sz="1100">
                     <a:solidFill>
-                      <a:schemeClr val="bg1"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:t>Steps</a:t>
@@ -3448,9 +3442,7 @@
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="tx2"/>
-        </a:solidFill>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -3461,9 +3453,7 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="tx2"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln>
       <a:noFill/>
     </a:ln>
@@ -3700,7 +3690,7 @@
             <a:r>
               <a:rPr lang="en-US" sz="1400" b="0" i="1">
                 <a:solidFill>
-                  <a:schemeClr val="bg1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:rPr>
               <a:t>Tags</a:t>
@@ -4000,7 +3990,7 @@
                 <a:r>
                   <a:rPr lang="en-US" sz="1100">
                     <a:solidFill>
-                      <a:schemeClr val="bg1"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:t>Scenarios</a:t>
@@ -4021,9 +4011,7 @@
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="tx2"/>
-        </a:solidFill>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -4034,9 +4022,7 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="tx2"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln>
       <a:noFill/>
     </a:ln>
@@ -4212,9 +4198,7 @@
               <a:prstGeom prst="rect">
                 <a:avLst/>
               </a:prstGeom>
-              <a:solidFill>
-                <a:schemeClr val="tx2"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="12700">
                 <a:solidFill>
                   <a:schemeClr val="dk1"/>
@@ -4274,9 +4258,7 @@
               <a:prstGeom prst="rect">
                 <a:avLst/>
               </a:prstGeom>
-              <a:solidFill>
-                <a:schemeClr val="tx2"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="12700">
                 <a:solidFill>
                   <a:schemeClr val="dk1"/>
@@ -4363,7 +4345,7 @@
                 <a:fld id="{07321330-A736-45CE-AAA5-68120F007E07}" type="TxLink">
                   <a:rPr lang="en-US" sz="1400" i="1">
                     <a:solidFill>
-                      <a:schemeClr val="accent6"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:pPr algn="ctr"/>
@@ -4371,7 +4353,7 @@
                 </a:fld>
                 <a:endParaRPr lang="en-US" sz="1400" i="1">
                   <a:solidFill>
-                    <a:schemeClr val="accent6"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                 </a:endParaRPr>
               </a:p>
@@ -4417,7 +4399,7 @@
                 <a:fld id="{C66D813D-5F81-41CE-8DAE-BBDD038F8F76}" type="TxLink">
                   <a:rPr lang="en-US" sz="1400" i="1">
                     <a:solidFill>
-                      <a:schemeClr val="accent6"/>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:pPr algn="ctr"/>
@@ -4425,7 +4407,7 @@
                 </a:fld>
                 <a:endParaRPr lang="en-US" sz="1400" i="1">
                   <a:solidFill>
-                    <a:schemeClr val="accent6"/>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                 </a:endParaRPr>
               </a:p>
@@ -4484,9 +4466,7 @@
                   <a:prstGeom prst="rect">
                     <a:avLst/>
                   </a:prstGeom>
-                  <a:solidFill>
-                    <a:schemeClr val="tx2"/>
-                  </a:solidFill>
+                  <a:noFill/>
                   <a:ln w="6350"/>
                 </xdr:spPr>
                 <xdr:style>
@@ -4551,24 +4531,20 @@
                       <a:prstGeom prst="roundRect">
                         <a:avLst/>
                       </a:prstGeom>
-                      <a:solidFill>
-                        <a:schemeClr val="bg1">
-                          <a:lumMod val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
+                      <a:ln w="3175"/>
                     </xdr:spPr>
                     <xdr:style>
-                      <a:lnRef idx="0">
-                        <a:schemeClr val="accent1"/>
+                      <a:lnRef idx="2">
+                        <a:schemeClr val="dk1"/>
                       </a:lnRef>
-                      <a:fillRef idx="3">
-                        <a:schemeClr val="accent1"/>
+                      <a:fillRef idx="1">
+                        <a:schemeClr val="lt1"/>
                       </a:fillRef>
-                      <a:effectRef idx="3">
-                        <a:schemeClr val="accent1"/>
+                      <a:effectRef idx="0">
+                        <a:schemeClr val="dk1"/>
                       </a:effectRef>
                       <a:fontRef idx="minor">
-                        <a:schemeClr val="lt1"/>
+                        <a:schemeClr val="dk1"/>
                       </a:fontRef>
                     </xdr:style>
                     <xdr:txBody>
@@ -4578,8 +4554,11 @@
                         <a:pPr algn="l"/>
                         <a:r>
                           <a:rPr lang="en-US" sz="1100">
+                            <a:ln>
+                              <a:noFill/>
+                            </a:ln>
                             <a:solidFill>
-                              <a:srgbClr val="51FF21"/>
+                              <a:schemeClr val="tx1"/>
                             </a:solidFill>
                           </a:rPr>
                           <a:t>PASSED</a:t>
@@ -4589,8 +4568,11 @@
                         <a:pPr algn="l"/>
                         <a:r>
                           <a:rPr lang="en-US" sz="1100">
+                            <a:ln>
+                              <a:noFill/>
+                            </a:ln>
                             <a:solidFill>
-                              <a:srgbClr val="FF0000"/>
+                              <a:schemeClr val="tx1"/>
                             </a:solidFill>
                           </a:rPr>
                           <a:t>FAILED</a:t>
@@ -4600,8 +4582,11 @@
                         <a:pPr algn="l"/>
                         <a:r>
                           <a:rPr lang="en-US" sz="1100">
+                            <a:ln>
+                              <a:noFill/>
+                            </a:ln>
                             <a:solidFill>
-                              <a:srgbClr val="FFFF00"/>
+                              <a:schemeClr val="tx1"/>
                             </a:solidFill>
                           </a:rPr>
                           <a:t>SKIPPED</a:t>
@@ -4611,6 +4596,9 @@
                         <a:pPr algn="l"/>
                         <a:r>
                           <a:rPr lang="en-US" sz="1100">
+                            <a:ln>
+                              <a:noFill/>
+                            </a:ln>
                             <a:solidFill>
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
@@ -4828,9 +4816,7 @@
                   <a:prstGeom prst="rect">
                     <a:avLst/>
                   </a:prstGeom>
-                  <a:solidFill>
-                    <a:schemeClr val="tx2"/>
-                  </a:solidFill>
+                  <a:noFill/>
                   <a:ln w="6350"/>
                 </xdr:spPr>
                 <xdr:style>
@@ -4869,24 +4855,20 @@
                   <a:prstGeom prst="roundRect">
                     <a:avLst/>
                   </a:prstGeom>
-                  <a:solidFill>
-                    <a:schemeClr val="bg1">
-                      <a:lumMod val="50000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
+                  <a:ln w="3175"/>
                 </xdr:spPr>
                 <xdr:style>
-                  <a:lnRef idx="0">
-                    <a:schemeClr val="accent1"/>
+                  <a:lnRef idx="2">
+                    <a:schemeClr val="dk1"/>
                   </a:lnRef>
-                  <a:fillRef idx="3">
-                    <a:schemeClr val="accent1"/>
+                  <a:fillRef idx="1">
+                    <a:schemeClr val="lt1"/>
                   </a:fillRef>
-                  <a:effectRef idx="3">
-                    <a:schemeClr val="accent1"/>
+                  <a:effectRef idx="0">
+                    <a:schemeClr val="dk1"/>
                   </a:effectRef>
                   <a:fontRef idx="minor">
-                    <a:schemeClr val="lt1"/>
+                    <a:schemeClr val="dk1"/>
                   </a:fontRef>
                 </xdr:style>
                 <xdr:txBody>
@@ -4905,7 +4887,7 @@
                     <a:r>
                       <a:rPr lang="en-US" sz="1200">
                         <a:solidFill>
-                          <a:srgbClr val="51FF21"/>
+                          <a:schemeClr val="tx1"/>
                         </a:solidFill>
                       </a:rPr>
                       <a:t>PASSED</a:t>
@@ -4916,7 +4898,7 @@
                     <a:r>
                       <a:rPr lang="en-US" sz="1200">
                         <a:solidFill>
-                          <a:srgbClr val="FF0000"/>
+                          <a:schemeClr val="tx1"/>
                         </a:solidFill>
                       </a:rPr>
                       <a:t>FAILED</a:t>
@@ -4927,7 +4909,7 @@
                     <a:r>
                       <a:rPr lang="en-US" sz="1200">
                         <a:solidFill>
-                          <a:srgbClr val="FFFF00"/>
+                          <a:schemeClr val="tx1"/>
                         </a:solidFill>
                       </a:rPr>
                       <a:t>SKIPPED</a:t>
@@ -5155,9 +5137,7 @@
                   <a:prstGeom prst="rect">
                     <a:avLst/>
                   </a:prstGeom>
-                  <a:solidFill>
-                    <a:schemeClr val="tx2"/>
-                  </a:solidFill>
+                  <a:noFill/>
                   <a:ln w="6350"/>
                 </xdr:spPr>
                 <xdr:style>
@@ -5196,24 +5176,20 @@
                   <a:prstGeom prst="roundRect">
                     <a:avLst/>
                   </a:prstGeom>
-                  <a:solidFill>
-                    <a:schemeClr val="bg1">
-                      <a:lumMod val="50000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
+                  <a:ln w="3175"/>
                 </xdr:spPr>
                 <xdr:style>
-                  <a:lnRef idx="0">
-                    <a:schemeClr val="accent1"/>
+                  <a:lnRef idx="2">
+                    <a:schemeClr val="dk1"/>
                   </a:lnRef>
-                  <a:fillRef idx="3">
-                    <a:schemeClr val="accent1"/>
+                  <a:fillRef idx="1">
+                    <a:schemeClr val="lt1"/>
                   </a:fillRef>
-                  <a:effectRef idx="3">
-                    <a:schemeClr val="accent1"/>
+                  <a:effectRef idx="0">
+                    <a:schemeClr val="dk1"/>
                   </a:effectRef>
                   <a:fontRef idx="minor">
-                    <a:schemeClr val="lt1"/>
+                    <a:schemeClr val="dk1"/>
                   </a:fontRef>
                 </xdr:style>
                 <xdr:txBody>
@@ -5232,7 +5208,7 @@
                     <a:r>
                       <a:rPr lang="en-US" sz="1100">
                         <a:solidFill>
-                          <a:srgbClr val="51FF21"/>
+                          <a:schemeClr val="tx1"/>
                         </a:solidFill>
                       </a:rPr>
                       <a:t>PASSED</a:t>
@@ -5243,7 +5219,7 @@
                     <a:r>
                       <a:rPr lang="en-US" sz="1100">
                         <a:solidFill>
-                          <a:srgbClr val="FF0000"/>
+                          <a:schemeClr val="tx1"/>
                         </a:solidFill>
                       </a:rPr>
                       <a:t>FAILED</a:t>
@@ -5254,7 +5230,7 @@
                     <a:r>
                       <a:rPr lang="en-US" sz="1100">
                         <a:solidFill>
-                          <a:srgbClr val="FFFF00"/>
+                          <a:schemeClr val="tx1"/>
                         </a:solidFill>
                       </a:rPr>
                       <a:t>SKIPPED</a:t>
@@ -5636,9 +5612,7 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:solidFill>
-              <a:schemeClr val="tx2"/>
-            </a:solidFill>
+            <a:noFill/>
             <a:ln w="12700">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
@@ -5726,7 +5700,7 @@
             <a:fld id="{ED1868E5-AE56-4ACA-8944-337939004EF9}" type="TxLink">
               <a:rPr lang="en-US" sz="2400" b="1" i="1" u="none" strike="noStrike">
                 <a:solidFill>
-                  <a:schemeClr val="accent6"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
@@ -5735,7 +5709,7 @@
             </a:fld>
             <a:endParaRPr lang="en-US" sz="2400" b="1" i="1">
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:endParaRPr>
           </a:p>
@@ -5895,7 +5869,7 @@
           <a:fld id="{790B2992-122F-4DED-8027-8C90CA641799}" type="TxLink">
             <a:rPr lang="en-US" sz="2400" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
@@ -5904,7 +5878,7 @@
           </a:fld>
           <a:endParaRPr lang="en-US" sz="2400" b="1">
             <a:solidFill>
-              <a:schemeClr val="accent6"/>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
           </a:endParaRPr>
         </a:p>
@@ -6062,7 +6036,7 @@
           <a:fld id="{55E37DD8-520B-4F7A-9381-E422E7073C87}" type="TxLink">
             <a:rPr lang="en-US" sz="3000" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
@@ -6071,7 +6045,7 @@
           </a:fld>
           <a:endParaRPr lang="en-US" sz="3000" b="1">
             <a:solidFill>
-              <a:schemeClr val="accent6"/>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
           </a:endParaRPr>
         </a:p>
@@ -6229,7 +6203,7 @@
           <a:fld id="{0C07208B-2D34-4675-9C99-827455C82BF1}" type="TxLink">
             <a:rPr lang="en-US" sz="2400" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
@@ -6238,7 +6212,7 @@
           </a:fld>
           <a:endParaRPr lang="en-US" sz="2400" b="1">
             <a:solidFill>
-              <a:schemeClr val="accent6"/>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
           </a:endParaRPr>
         </a:p>
@@ -6338,24 +6312,20 @@
         <a:prstGeom prst="roundRect">
           <a:avLst/>
         </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:ln w="3175"/>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0">
-          <a:schemeClr val="accent1"/>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
         </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
         </a:fillRef>
-        <a:effectRef idx="3">
-          <a:schemeClr val="accent1"/>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="dk1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
@@ -6366,7 +6336,7 @@
           <a:r>
             <a:rPr lang="en-US" sz="1200">
               <a:solidFill>
-                <a:srgbClr val="51FF21"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
             <a:t>PASSED</a:t>
@@ -6377,7 +6347,7 @@
           <a:r>
             <a:rPr lang="en-US" sz="1200">
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
             <a:t>FAILED</a:t>
@@ -6388,7 +6358,7 @@
           <a:r>
             <a:rPr lang="en-US" sz="1200">
               <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
             <a:t>SKIPPED</a:t>
@@ -6903,24 +6873,20 @@
         <a:prstGeom prst="roundRect">
           <a:avLst/>
         </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:ln w="3175"/>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0">
-          <a:schemeClr val="accent1"/>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
         </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
         </a:fillRef>
-        <a:effectRef idx="3">
-          <a:schemeClr val="accent1"/>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="dk1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
@@ -6931,7 +6897,7 @@
           <a:r>
             <a:rPr lang="en-US" sz="1200">
               <a:solidFill>
-                <a:srgbClr val="51FF21"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
             <a:t>PASSED</a:t>
@@ -6942,7 +6908,7 @@
           <a:r>
             <a:rPr lang="en-US" sz="1200">
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
             <a:t>FAILED</a:t>
@@ -6953,7 +6919,7 @@
           <a:r>
             <a:rPr lang="en-US" sz="1200">
               <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
             <a:t>SKIPPED</a:t>
@@ -8081,9 +8047,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>